<commit_message>
Fixed one-based index with Excel parser.
</commit_message>
<xml_diff>
--- a/TewlTester/TestFiles/TewlTestBook.xlsx
+++ b/TewlTester/TestFiles/TewlTestBook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EveryoneFullControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\TEWL\TewlTester\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A79FF6EE-A7E2-4CCF-8123-D8D05F21E9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DFBB54-94CD-4E29-9BE9-B886FA8B5689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="3795" windowWidth="25935" windowHeight="13635" xr2:uid="{C0804DFD-4032-4BE1-89B4-F2029E39EC5F}"/>
   </bookViews>
@@ -44,34 +44,34 @@
     <t>Date</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Don</t>
+  </si>
+  <si>
+    <t>Hilda</t>
+  </si>
+  <si>
+    <t>Fran</t>
+  </si>
+  <si>
+    <t>Eddie</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Owen</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added write tests. Changed Date detection for Excel file writer to be more lenient.
</commit_message>
<xml_diff>
--- a/TewlTester/TestFiles/TewlTestBook.xlsx
+++ b/TewlTester/TestFiles/TewlTestBook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\TEWL\TewlTester\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TEWL\TewlTester\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DFBB54-94CD-4E29-9BE9-B886FA8B5689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD4F11E-FB5D-4924-B3DC-6A225AD86E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3795" windowWidth="25935" windowHeight="13635" xr2:uid="{C0804DFD-4032-4BE1-89B4-F2029E39EC5F}"/>
+    <workbookView xWindow="8580" yWindow="3015" windowWidth="28800" windowHeight="15345" xr2:uid="{C0804DFD-4032-4BE1-89B4-F2029E39EC5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -72,13 +72,25 @@
   </si>
   <si>
     <t>Owen</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>greg.smalter@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +100,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,14 +130,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C5B44D-3BF6-4A52-A801-0DB79E08D5A0}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +465,7 @@
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +475,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,7 +493,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -474,8 +503,11 @@
       <c r="C3" s="1">
         <v>43862</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -486,7 +518,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -497,7 +529,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -507,8 +539,11 @@
       <c r="C6" s="1">
         <v>43952</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -519,7 +554,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -530,7 +565,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -541,7 +576,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -552,7 +587,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -565,6 +600,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{3DFC4AA6-ACF0-4D38-BE73-62C0C271D3D3}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{8D66F164-5EED-4C74-85A2-C88686518A65}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>